<commit_message>
close review Point for team x
</commit_message>
<xml_diff>
--- a/Review X/PO_SAG_DOC_Team_X_Review.xlsx
+++ b/Review X/PO_SAG_DOC_Team_X_Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation Project\github_repos\GraduationProjectDocumentation\Review X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B73E95E-5948-4921-9E6E-D566938FA302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984E572E-6C30-4D7B-B590-2795846EC4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>Entry Date</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>DocType_REV_ID</t>
@@ -115,9 +112,6 @@
     <t>DOC_REVIEW_006</t>
   </si>
   <si>
-    <t>DOC_REVIEW_007</t>
-  </si>
-  <si>
     <t>6//Abstract/ paragraph 6</t>
   </si>
   <si>
@@ -134,12 +128,6 @@
   </si>
   <si>
     <t>6//Abstract/ paragraph 7</t>
-  </si>
-  <si>
-    <t>reading signs isn't one of our features</t>
-  </si>
-  <si>
-    <t>Signs is out of scope (not match our detected objects)</t>
   </si>
   <si>
     <t>6//Abstract/paragraph 7</t>
@@ -189,6 +177,9 @@
   </si>
   <si>
     <t>Conclusion should be added</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -302,30 +293,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b/>
@@ -632,10 +600,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -650,7 +618,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -668,7 +636,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -676,334 +644,308 @@
     </row>
     <row r="2" spans="1:8" ht="103.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4">
         <v>44572</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4">
         <v>44572</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="72" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4">
         <v>44572</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4">
         <v>44572</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4">
         <v>44572</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4">
         <v>44572</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4">
         <v>44572</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>6</v>
+      <c r="H8" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4">
         <v>44572</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="52.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4">
         <v>44572</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="F10" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="52.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4">
         <v>44572</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="52.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="4">
-        <v>44572</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:H9">
-    <cfRule type="expression" dxfId="9" priority="11">
+  <conditionalFormatting sqref="A2:H8">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H9">
-    <cfRule type="expression" dxfId="8" priority="12">
+  <conditionalFormatting sqref="A2:H8">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H9">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$H9 = "Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H9">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$H9= "Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A10:H10">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$H10 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:H10">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$H10= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:H11">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$H11 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:H11">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$H11= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:H12">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$H12 = "Closed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:H12">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$H12= "Open"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>